<commit_message>
lots of updates, minimal progress
</commit_message>
<xml_diff>
--- a/Specific aim 2/Practice MPT/naveirmd_start_table.xlsx
+++ b/Specific aim 2/Practice MPT/naveirmd_start_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/90280e413f276f71/Documents/GitHub/DR2/Specific aim 2/Practice MPT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3E1E99DA-9F2C-48C7-88AE-AD3B478D7674}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="8_{3E1E99DA-9F2C-48C7-88AE-AD3B478D7674}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1F588C9A-79D5-40EE-9274-46B1E43A5E1D}"/>
   <bookViews>
-    <workbookView xWindow="42675" yWindow="3210" windowWidth="25185" windowHeight="13350" xr2:uid="{827B344C-D30C-44B8-86BF-D45C0EAD0B5F}"/>
+    <workbookView xWindow="28680" yWindow="-75" windowWidth="29040" windowHeight="15840" xr2:uid="{827B344C-D30C-44B8-86BF-D45C0EAD0B5F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,9 +39,6 @@
     <t>trial</t>
   </si>
   <si>
-    <t>item</t>
-  </si>
-  <si>
     <t>person</t>
   </si>
   <si>
@@ -55,6 +52,9 @@
   </si>
   <si>
     <t>y</t>
+  </si>
+  <si>
+    <t>item</t>
   </si>
 </sst>
 </file>
@@ -406,43 +406,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ECFF369-B481-4977-8B6E-F3BCDDD5FD62}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B33" sqref="B2:B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>273</v>
+        <v>5</v>
       </c>
       <c r="B2">
-        <v>5</v>
+        <v>123</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -462,10 +462,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>273</v>
+        <v>5</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>123</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -485,10 +485,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>273</v>
+        <v>5</v>
       </c>
       <c r="B4">
-        <v>5</v>
+        <v>123</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -508,10 +508,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>273</v>
+        <v>5</v>
       </c>
       <c r="B5">
-        <v>5</v>
+        <v>123</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -531,10 +531,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>273</v>
+        <v>5</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>123</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -554,10 +554,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>273</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>5</v>
+        <v>123</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -577,10 +577,10 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>273</v>
+        <v>5</v>
       </c>
       <c r="B8">
-        <v>5</v>
+        <v>123</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -600,10 +600,10 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>273</v>
+        <v>5</v>
       </c>
       <c r="B9">
-        <v>5</v>
+        <v>123</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -618,6 +618,558 @@
         <v>0.5</v>
       </c>
       <c r="G9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="B10">
+        <v>123</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>180</v>
+      </c>
+      <c r="E10">
+        <v>0.5</v>
+      </c>
+      <c r="F10">
+        <v>0.5</v>
+      </c>
+      <c r="G10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>6</v>
+      </c>
+      <c r="B11">
+        <v>123</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>190</v>
+      </c>
+      <c r="E11">
+        <v>0.5</v>
+      </c>
+      <c r="F11">
+        <v>0.5</v>
+      </c>
+      <c r="G11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>6</v>
+      </c>
+      <c r="B12">
+        <v>123</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>200</v>
+      </c>
+      <c r="E12">
+        <v>0.5</v>
+      </c>
+      <c r="F12">
+        <v>0.5</v>
+      </c>
+      <c r="G12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>6</v>
+      </c>
+      <c r="B13">
+        <v>123</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>210</v>
+      </c>
+      <c r="E13">
+        <v>0.5</v>
+      </c>
+      <c r="F13">
+        <v>0.5</v>
+      </c>
+      <c r="G13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>6</v>
+      </c>
+      <c r="B14">
+        <v>123</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>220</v>
+      </c>
+      <c r="E14">
+        <v>0.5</v>
+      </c>
+      <c r="F14">
+        <v>0.5</v>
+      </c>
+      <c r="G14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>6</v>
+      </c>
+      <c r="B15">
+        <v>123</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>230</v>
+      </c>
+      <c r="E15">
+        <v>0.5</v>
+      </c>
+      <c r="F15">
+        <v>0.5</v>
+      </c>
+      <c r="G15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>6</v>
+      </c>
+      <c r="B16">
+        <v>123</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>240</v>
+      </c>
+      <c r="E16">
+        <v>0.5</v>
+      </c>
+      <c r="F16">
+        <v>0.5</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>6</v>
+      </c>
+      <c r="B17">
+        <v>123</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>250</v>
+      </c>
+      <c r="E17">
+        <v>0.5</v>
+      </c>
+      <c r="F17">
+        <v>0.5</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>5</v>
+      </c>
+      <c r="B18">
+        <v>123</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <v>180</v>
+      </c>
+      <c r="E18">
+        <v>0.5</v>
+      </c>
+      <c r="F18">
+        <v>0.5</v>
+      </c>
+      <c r="G18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>5</v>
+      </c>
+      <c r="B19">
+        <v>123</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>190</v>
+      </c>
+      <c r="E19">
+        <v>0.5</v>
+      </c>
+      <c r="F19">
+        <v>0.5</v>
+      </c>
+      <c r="G19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>5</v>
+      </c>
+      <c r="B20">
+        <v>123</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20">
+        <v>200</v>
+      </c>
+      <c r="E20">
+        <v>0.5</v>
+      </c>
+      <c r="F20">
+        <v>0.5</v>
+      </c>
+      <c r="G20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>5</v>
+      </c>
+      <c r="B21">
+        <v>123</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21">
+        <v>210</v>
+      </c>
+      <c r="E21">
+        <v>0.5</v>
+      </c>
+      <c r="F21">
+        <v>0.5</v>
+      </c>
+      <c r="G21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>5</v>
+      </c>
+      <c r="B22">
+        <v>123</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22">
+        <v>220</v>
+      </c>
+      <c r="E22">
+        <v>0.5</v>
+      </c>
+      <c r="F22">
+        <v>0.5</v>
+      </c>
+      <c r="G22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>5</v>
+      </c>
+      <c r="B23">
+        <v>123</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23">
+        <v>230</v>
+      </c>
+      <c r="E23">
+        <v>0.5</v>
+      </c>
+      <c r="F23">
+        <v>0.5</v>
+      </c>
+      <c r="G23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>5</v>
+      </c>
+      <c r="B24">
+        <v>123</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24">
+        <v>240</v>
+      </c>
+      <c r="E24">
+        <v>0.5</v>
+      </c>
+      <c r="F24">
+        <v>0.5</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>5</v>
+      </c>
+      <c r="B25">
+        <v>123</v>
+      </c>
+      <c r="C25">
+        <v>2</v>
+      </c>
+      <c r="D25">
+        <v>250</v>
+      </c>
+      <c r="E25">
+        <v>0.5</v>
+      </c>
+      <c r="F25">
+        <v>0.5</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>6</v>
+      </c>
+      <c r="B26">
+        <v>123</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26">
+        <v>180</v>
+      </c>
+      <c r="E26">
+        <v>0.5</v>
+      </c>
+      <c r="F26">
+        <v>0.5</v>
+      </c>
+      <c r="G26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>6</v>
+      </c>
+      <c r="B27">
+        <v>123</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+      <c r="D27">
+        <v>190</v>
+      </c>
+      <c r="E27">
+        <v>0.5</v>
+      </c>
+      <c r="F27">
+        <v>0.5</v>
+      </c>
+      <c r="G27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>6</v>
+      </c>
+      <c r="B28">
+        <v>123</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28">
+        <v>200</v>
+      </c>
+      <c r="E28">
+        <v>0.5</v>
+      </c>
+      <c r="F28">
+        <v>0.5</v>
+      </c>
+      <c r="G28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>6</v>
+      </c>
+      <c r="B29">
+        <v>123</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29">
+        <v>210</v>
+      </c>
+      <c r="E29">
+        <v>0.5</v>
+      </c>
+      <c r="F29">
+        <v>0.5</v>
+      </c>
+      <c r="G29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>6</v>
+      </c>
+      <c r="B30">
+        <v>123</v>
+      </c>
+      <c r="C30">
+        <v>2</v>
+      </c>
+      <c r="D30">
+        <v>220</v>
+      </c>
+      <c r="E30">
+        <v>0.5</v>
+      </c>
+      <c r="F30">
+        <v>0.5</v>
+      </c>
+      <c r="G30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>6</v>
+      </c>
+      <c r="B31">
+        <v>123</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="D31">
+        <v>230</v>
+      </c>
+      <c r="E31">
+        <v>0.5</v>
+      </c>
+      <c r="F31">
+        <v>0.5</v>
+      </c>
+      <c r="G31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>6</v>
+      </c>
+      <c r="B32">
+        <v>123</v>
+      </c>
+      <c r="C32">
+        <v>2</v>
+      </c>
+      <c r="D32">
+        <v>240</v>
+      </c>
+      <c r="E32">
+        <v>0.5</v>
+      </c>
+      <c r="F32">
+        <v>0.5</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>6</v>
+      </c>
+      <c r="B33">
+        <v>123</v>
+      </c>
+      <c r="C33">
+        <v>2</v>
+      </c>
+      <c r="D33">
+        <v>250</v>
+      </c>
+      <c r="E33">
+        <v>0.5</v>
+      </c>
+      <c r="F33">
+        <v>0.5</v>
+      </c>
+      <c r="G33">
         <v>1</v>
       </c>
     </row>

</xml_diff>